<commit_message>
L2S and S2l Scenarios
</commit_message>
<xml_diff>
--- a/cypress/fixtures/SkavaMessageContracts.xlsx
+++ b/cypress/fixtures/SkavaMessageContracts.xlsx
@@ -17,10 +17,11 @@
     <sheet state="visible" name="YLAccountSubscription" sheetId="12" r:id="rId15"/>
     <sheet state="visible" name="YLAccountUpdated" sheetId="13" r:id="rId16"/>
     <sheet state="visible" name="YLCustomerAddressUpdated" sheetId="14" r:id="rId17"/>
-    <sheet state="visible" name="SkavaAccount" sheetId="15" r:id="rId18"/>
-    <sheet state="visible" name="OrderPlacedProcessed" sheetId="16" r:id="rId19"/>
-    <sheet state="visible" name="OrderReplacedProcessed" sheetId="17" r:id="rId20"/>
-    <sheet state="visible" name="OrderReturnedProcessed" sheetId="18" r:id="rId21"/>
+    <sheet state="visible" name="SkavaAccountProcessed" sheetId="15" r:id="rId18"/>
+    <sheet state="visible" name="SkavaCustomerAddressProcessed" sheetId="16" r:id="rId19"/>
+    <sheet state="visible" name="OrderPlacedProcessed" sheetId="17" r:id="rId20"/>
+    <sheet state="visible" name="OrderReplacedProcessed" sheetId="18" r:id="rId21"/>
+    <sheet state="visible" name="OrderReturnedProcessed" sheetId="19" r:id="rId22"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1032" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="295">
   <si>
     <t>Name</t>
   </si>
@@ -1047,7 +1048,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1114,6 +1115,9 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1168,6 +1172,10 @@
 </file>
 
 <file path=xl/drawings/drawing18.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing19.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2555,9 +2563,6 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="15.63"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -2571,75 +2576,49 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="20" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="20" t="s">
+        <v>285</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="22"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="20" t="s">
         <v>288</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="24"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="14" t="s">
-        <v>287</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="24"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="B7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="15" t="s">
+      <c r="B5" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>7</v>
       </c>
     </row>
@@ -2657,6 +2636,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="15.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -2671,21 +2653,19 @@
     </row>
     <row r="2">
       <c r="A2" s="14" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="15" t="s">
-        <v>7</v>
-      </c>
+      <c r="C2" s="25"/>
     </row>
     <row r="3">
       <c r="A3" s="14" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>6</v>
+        <v>174</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>7</v>
@@ -2693,10 +2673,10 @@
     </row>
     <row r="4">
       <c r="A4" s="14" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>174</v>
+        <v>4</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>7</v>
@@ -2704,12 +2684,45 @@
     </row>
     <row r="5">
       <c r="A5" s="14" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14" t="s">
+        <v>291</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="25"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="14" t="s">
+        <v>293</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2727,13 +2740,81 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="17"/>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>